<commit_message>
Showcase of DDT features
</commit_message>
<xml_diff>
--- a/OpenMRS_DDT/Main.rvl.xlsx
+++ b/OpenMRS_DDT/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="71">
   <si>
     <t>Flow</t>
   </si>
@@ -208,6 +208,24 @@
   </si>
   <si>
     <t>%WORKDIR%\RegisterPatient\Main.rvl.xlsx</t>
+  </si>
+  <si>
+    <t>DoPlayTest</t>
+  </si>
+  <si>
+    <t>pathToTest</t>
+  </si>
+  <si>
+    <t>%WORKDIR%\DataOrigin\DataOrigin.sstest</t>
+  </si>
+  <si>
+    <t>%WORKDIR%\DataSources\Main.rvl.xlsx</t>
+  </si>
+  <si>
+    <t>%WORKDIR%\DataOrigin\Main.rvl.xlsx</t>
+  </si>
+  <si>
+    <t>%WORKDIR%\DataOutput\Main.rvl.xlsx</t>
   </si>
 </sst>
 </file>
@@ -857,33 +875,71 @@
       <c r="H6" s="56"/>
     </row>
     <row r="7">
-      <c r="A7" s="57"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63"/>
+      <c r="A7" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>68</v>
+      </c>
       <c r="H7" s="64"/>
     </row>
     <row r="8">
       <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="71"/>
+      <c r="B8" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="70" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="71" t="s">
+        <v>69</v>
+      </c>
       <c r="H8" s="72"/>
     </row>
     <row r="9">
       <c r="A9" s="73"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="77"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="79"/>
+      <c r="B9" s="74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="79" t="s">
+        <v>70</v>
+      </c>
       <c r="H9" s="80"/>
     </row>
     <row r="10">

</xml_diff>